<commit_message>
versao completa e testada
</commit_message>
<xml_diff>
--- a/PLANILHA PROPOSTA R2 OFICIAL.xlsx
+++ b/PLANILHA PROPOSTA R2 OFICIAL.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f3978efb2e6b0e4/Área de Trabalho/SISTEMA RESOLVI 2.7 FIXED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Vitor\Desktop\SISTEMA RESOLVI DEFINITIVO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{A996D06F-25E3-4CDF-B7C8-C23028876438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F99304B5-5C33-4B0E-B926-52A41B17E568}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="135" windowWidth="16380" windowHeight="15465" xr2:uid="{B1930526-7FBF-4CB4-AF6F-8488152F940F}"/>
+    <workbookView xWindow="15" yWindow="135" windowWidth="16380" windowHeight="15465"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>MODELO DE PROPOSTA DE PREÇOS</t>
   </si>
@@ -70,9 +69,6 @@
     </r>
   </si>
   <si>
-    <t>planilha de itens:</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -94,9 +90,6 @@
     <t>Valor Total</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t xml:space="preserve">Declaramos que estamos ciente e concordamos com as condições contidas no edital e seus anexos, bem como de que a proposta apresentada compreende a integralidade dos custos para atendimento dos direitos trabalhistas assegurados na Constituição Federal, nas leis trabalhistas, nas normas infralegais, nas convenções coletivas de trabalho e nos termos de ajustamento de conduta vigentes na data de sua entrega em definitivo e que cumpre plenamente os requisitos de habilitação definidos no instrumento convocatório. </t>
   </si>
   <si>
@@ -140,16 +133,20 @@
   </si>
   <si>
     <t>NUMERO DO PREGAO</t>
+  </si>
+  <si>
+    <t>Planilha de Itens:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +170,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -188,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -211,22 +222,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -234,24 +233,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -259,23 +275,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -587,11 +589,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3AB193-8E09-464A-872E-9D3CB710D640}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,371 +608,495 @@
   </cols>
   <sheetData>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="12"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="4" t="s">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7">
-        <f>F21*E21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7">
-        <f t="shared" ref="G22:G24" si="0">F22*E22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="3">
-        <f>SUM(G21:G24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="B55" s="15"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="14"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="16"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="12" t="s">
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="12" t="s">
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+    </row>
+    <row r="67" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
-    </row>
-    <row r="67" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
-      <c r="G70" s="12"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
+      <c r="A73" s="13"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
+      <c r="A74" s="16"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="22">
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="A68:G68"/>
+    <mergeCell ref="A69:G69"/>
+    <mergeCell ref="A70:G70"/>
+    <mergeCell ref="A71:G71"/>
+    <mergeCell ref="A72:G72"/>
+    <mergeCell ref="A73:G73"/>
     <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A25:F25"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="A13:B13"/>
@@ -985,13 +1111,6 @@
     <mergeCell ref="A64:G64"/>
     <mergeCell ref="A65:G65"/>
     <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="A68:G68"/>
-    <mergeCell ref="A69:G69"/>
-    <mergeCell ref="A70:G70"/>
-    <mergeCell ref="A71:G71"/>
-    <mergeCell ref="A72:G72"/>
-    <mergeCell ref="A73:G73"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.35433070866141736" bottom="2.3228346456692917" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>